<commit_message>
Deleted old SameDiffSents materials and data, continued converting SameDiffSents to AgentPatientStimuli
</commit_message>
<xml_diff>
--- a/RealLangStims/OrdersAP/info_A1.xlsx
+++ b/RealLangStims/OrdersAP/info_A1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilyjordan/Desktop/EvLab/GitHub stuff/AgentPatientStimuli/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilyjordan/Desktop/EvLab/GitHub stuff/AgentPatientStimuli/RealLangStims/OrdersAP/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="8">
   <si>
     <t>Onset</t>
   </si>
@@ -46,15 +46,25 @@
   <si>
     <t>Patient</t>
   </si>
+  <si>
+    <t>#Onset and duration not randomized yet - copied from a sample optseq</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -80,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,15 +370,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E121"/>
+  <dimension ref="A1:F121"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E121"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="59.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -383,11 +397,20 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>6</v>
+      </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -395,10 +418,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
       <c r="D3" t="s">
         <v>5</v>
       </c>
@@ -406,10 +435,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="1">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
@@ -417,10 +452,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" s="1">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
@@ -428,10 +469,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="1">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
@@ -439,10 +486,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" s="1">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4</v>
+      </c>
       <c r="D7" t="s">
         <v>5</v>
       </c>
@@ -450,10 +503,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" s="1">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1">
+        <v>6</v>
+      </c>
       <c r="D8" t="s">
         <v>5</v>
       </c>
@@ -461,10 +520,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" s="1">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1">
+        <v>6</v>
+      </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
@@ -472,10 +537,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" s="1">
+        <v>38</v>
+      </c>
+      <c r="C10" s="1">
+        <v>2</v>
+      </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
@@ -483,10 +554,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" s="1">
+        <v>40</v>
+      </c>
+      <c r="C11" s="1">
+        <v>6</v>
+      </c>
       <c r="D11" t="s">
         <v>5</v>
       </c>
@@ -494,10 +571,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" s="1">
+        <v>46</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2</v>
+      </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
@@ -505,10 +588,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" s="1">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6</v>
+      </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
@@ -516,10 +605,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" s="1">
+        <v>54</v>
+      </c>
+      <c r="C14" s="1">
+        <v>6</v>
+      </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
@@ -527,10 +622,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" s="1">
+        <v>60</v>
+      </c>
+      <c r="C15" s="1">
+        <v>6</v>
+      </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
@@ -538,9 +639,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>66</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
@@ -553,6 +660,12 @@
       <c r="A17">
         <v>16</v>
       </c>
+      <c r="B17" s="1">
+        <v>72</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
@@ -564,6 +677,12 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" s="1">
+        <v>78</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
       <c r="D18" t="s">
         <v>5</v>
       </c>
@@ -575,6 +694,12 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" s="1">
+        <v>84</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
       <c r="D19" t="s">
         <v>5</v>
       </c>
@@ -586,6 +711,12 @@
       <c r="A20">
         <v>19</v>
       </c>
+      <c r="B20" s="1">
+        <v>90</v>
+      </c>
+      <c r="C20" s="1">
+        <v>6</v>
+      </c>
       <c r="D20" t="s">
         <v>5</v>
       </c>
@@ -597,6 +728,12 @@
       <c r="A21">
         <v>20</v>
       </c>
+      <c r="B21" s="1">
+        <v>96</v>
+      </c>
+      <c r="C21" s="1">
+        <v>6</v>
+      </c>
       <c r="D21" t="s">
         <v>5</v>
       </c>
@@ -608,6 +745,12 @@
       <c r="A22">
         <v>21</v>
       </c>
+      <c r="B22" s="1">
+        <v>102</v>
+      </c>
+      <c r="C22" s="1">
+        <v>2</v>
+      </c>
       <c r="D22" t="s">
         <v>5</v>
       </c>
@@ -619,6 +762,12 @@
       <c r="A23">
         <v>22</v>
       </c>
+      <c r="B23" s="1">
+        <v>104</v>
+      </c>
+      <c r="C23" s="1">
+        <v>6</v>
+      </c>
       <c r="D23" t="s">
         <v>5</v>
       </c>
@@ -630,6 +779,12 @@
       <c r="A24">
         <v>23</v>
       </c>
+      <c r="B24" s="1">
+        <v>110</v>
+      </c>
+      <c r="C24" s="1">
+        <v>6</v>
+      </c>
       <c r="D24" t="s">
         <v>5</v>
       </c>
@@ -641,6 +796,12 @@
       <c r="A25">
         <v>24</v>
       </c>
+      <c r="B25" s="1">
+        <v>116</v>
+      </c>
+      <c r="C25" s="1">
+        <v>4</v>
+      </c>
       <c r="D25" t="s">
         <v>5</v>
       </c>
@@ -652,6 +813,12 @@
       <c r="A26">
         <v>25</v>
       </c>
+      <c r="B26" s="1">
+        <v>120</v>
+      </c>
+      <c r="C26" s="1">
+        <v>6</v>
+      </c>
       <c r="D26" t="s">
         <v>5</v>
       </c>
@@ -663,6 +830,12 @@
       <c r="A27">
         <v>26</v>
       </c>
+      <c r="B27" s="1">
+        <v>126</v>
+      </c>
+      <c r="C27" s="1">
+        <v>4</v>
+      </c>
       <c r="D27" t="s">
         <v>5</v>
       </c>
@@ -674,6 +847,12 @@
       <c r="A28">
         <v>27</v>
       </c>
+      <c r="B28" s="1">
+        <v>130</v>
+      </c>
+      <c r="C28" s="1">
+        <v>6</v>
+      </c>
       <c r="D28" t="s">
         <v>5</v>
       </c>
@@ -685,6 +864,12 @@
       <c r="A29">
         <v>28</v>
       </c>
+      <c r="B29" s="1">
+        <v>136</v>
+      </c>
+      <c r="C29" s="1">
+        <v>4</v>
+      </c>
       <c r="D29" t="s">
         <v>5</v>
       </c>
@@ -696,6 +881,12 @@
       <c r="A30">
         <v>29</v>
       </c>
+      <c r="B30" s="1">
+        <v>140</v>
+      </c>
+      <c r="C30" s="1">
+        <v>6</v>
+      </c>
       <c r="D30" t="s">
         <v>5</v>
       </c>
@@ -707,6 +898,12 @@
       <c r="A31">
         <v>30</v>
       </c>
+      <c r="B31" s="1">
+        <v>146</v>
+      </c>
+      <c r="C31" s="1">
+        <v>4</v>
+      </c>
       <c r="D31" t="s">
         <v>5</v>
       </c>
@@ -718,6 +915,12 @@
       <c r="A32">
         <v>31</v>
       </c>
+      <c r="B32" s="1">
+        <v>150</v>
+      </c>
+      <c r="C32" s="1">
+        <v>6</v>
+      </c>
       <c r="D32" t="s">
         <v>5</v>
       </c>
@@ -729,6 +932,12 @@
       <c r="A33">
         <v>32</v>
       </c>
+      <c r="B33" s="1">
+        <v>156</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2</v>
+      </c>
       <c r="D33" t="s">
         <v>5</v>
       </c>
@@ -740,6 +949,12 @@
       <c r="A34">
         <v>33</v>
       </c>
+      <c r="B34" s="1">
+        <v>158</v>
+      </c>
+      <c r="C34" s="1">
+        <v>6</v>
+      </c>
       <c r="D34" t="s">
         <v>5</v>
       </c>
@@ -751,6 +966,12 @@
       <c r="A35">
         <v>34</v>
       </c>
+      <c r="B35" s="1">
+        <v>164</v>
+      </c>
+      <c r="C35" s="1">
+        <v>6</v>
+      </c>
       <c r="D35" t="s">
         <v>5</v>
       </c>
@@ -762,6 +983,12 @@
       <c r="A36">
         <v>35</v>
       </c>
+      <c r="B36" s="1">
+        <v>170</v>
+      </c>
+      <c r="C36" s="1">
+        <v>6</v>
+      </c>
       <c r="D36" t="s">
         <v>5</v>
       </c>
@@ -773,6 +1000,12 @@
       <c r="A37">
         <v>36</v>
       </c>
+      <c r="B37" s="1">
+        <v>176</v>
+      </c>
+      <c r="C37" s="1">
+        <v>6</v>
+      </c>
       <c r="D37" t="s">
         <v>5</v>
       </c>
@@ -784,6 +1017,12 @@
       <c r="A38">
         <v>37</v>
       </c>
+      <c r="B38" s="1">
+        <v>182</v>
+      </c>
+      <c r="C38" s="1">
+        <v>6</v>
+      </c>
       <c r="D38" t="s">
         <v>5</v>
       </c>
@@ -795,6 +1034,12 @@
       <c r="A39">
         <v>38</v>
       </c>
+      <c r="B39" s="1">
+        <v>188</v>
+      </c>
+      <c r="C39" s="1">
+        <v>6</v>
+      </c>
       <c r="D39" t="s">
         <v>5</v>
       </c>
@@ -806,6 +1051,12 @@
       <c r="A40">
         <v>39</v>
       </c>
+      <c r="B40" s="1">
+        <v>194</v>
+      </c>
+      <c r="C40" s="1">
+        <v>6</v>
+      </c>
       <c r="D40" t="s">
         <v>5</v>
       </c>
@@ -817,6 +1068,12 @@
       <c r="A41">
         <v>40</v>
       </c>
+      <c r="B41" s="1">
+        <v>200</v>
+      </c>
+      <c r="C41" s="1">
+        <v>8</v>
+      </c>
       <c r="D41" t="s">
         <v>5</v>
       </c>
@@ -828,6 +1085,12 @@
       <c r="A42">
         <v>41</v>
       </c>
+      <c r="B42" s="1">
+        <v>208</v>
+      </c>
+      <c r="C42" s="1">
+        <v>6</v>
+      </c>
       <c r="D42" t="s">
         <v>5</v>
       </c>
@@ -839,6 +1102,12 @@
       <c r="A43">
         <v>42</v>
       </c>
+      <c r="B43" s="1">
+        <v>214</v>
+      </c>
+      <c r="C43" s="1">
+        <v>6</v>
+      </c>
       <c r="D43" t="s">
         <v>5</v>
       </c>
@@ -850,6 +1119,12 @@
       <c r="A44">
         <v>43</v>
       </c>
+      <c r="B44" s="1">
+        <v>220</v>
+      </c>
+      <c r="C44" s="1">
+        <v>2</v>
+      </c>
       <c r="D44" t="s">
         <v>5</v>
       </c>
@@ -861,6 +1136,12 @@
       <c r="A45">
         <v>44</v>
       </c>
+      <c r="B45" s="1">
+        <v>222</v>
+      </c>
+      <c r="C45" s="1">
+        <v>6</v>
+      </c>
       <c r="D45" t="s">
         <v>5</v>
       </c>
@@ -872,6 +1153,12 @@
       <c r="A46">
         <v>45</v>
       </c>
+      <c r="B46" s="1">
+        <v>228</v>
+      </c>
+      <c r="C46" s="1">
+        <v>2</v>
+      </c>
       <c r="D46" t="s">
         <v>5</v>
       </c>
@@ -883,6 +1170,12 @@
       <c r="A47">
         <v>46</v>
       </c>
+      <c r="B47" s="1">
+        <v>230</v>
+      </c>
+      <c r="C47" s="1">
+        <v>6</v>
+      </c>
       <c r="D47" t="s">
         <v>5</v>
       </c>
@@ -894,6 +1187,12 @@
       <c r="A48">
         <v>47</v>
       </c>
+      <c r="B48" s="1">
+        <v>236</v>
+      </c>
+      <c r="C48" s="1">
+        <v>4</v>
+      </c>
       <c r="D48" t="s">
         <v>5</v>
       </c>
@@ -905,6 +1204,12 @@
       <c r="A49">
         <v>48</v>
       </c>
+      <c r="B49" s="1">
+        <v>240</v>
+      </c>
+      <c r="C49" s="1">
+        <v>6</v>
+      </c>
       <c r="D49" t="s">
         <v>5</v>
       </c>
@@ -916,6 +1221,12 @@
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" s="1">
+        <v>246</v>
+      </c>
+      <c r="C50" s="1">
+        <v>6</v>
+      </c>
       <c r="D50" t="s">
         <v>5</v>
       </c>
@@ -927,6 +1238,12 @@
       <c r="A51">
         <v>50</v>
       </c>
+      <c r="B51" s="1">
+        <v>252</v>
+      </c>
+      <c r="C51" s="1">
+        <v>6</v>
+      </c>
       <c r="D51" t="s">
         <v>5</v>
       </c>
@@ -938,6 +1255,12 @@
       <c r="A52">
         <v>51</v>
       </c>
+      <c r="B52" s="1">
+        <v>258</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4</v>
+      </c>
       <c r="D52" t="s">
         <v>5</v>
       </c>
@@ -949,6 +1272,12 @@
       <c r="A53">
         <v>52</v>
       </c>
+      <c r="B53" s="1">
+        <v>262</v>
+      </c>
+      <c r="C53" s="1">
+        <v>6</v>
+      </c>
       <c r="D53" t="s">
         <v>5</v>
       </c>
@@ -960,6 +1289,12 @@
       <c r="A54">
         <v>53</v>
       </c>
+      <c r="B54" s="1">
+        <v>268</v>
+      </c>
+      <c r="C54" s="1">
+        <v>6</v>
+      </c>
       <c r="D54" t="s">
         <v>5</v>
       </c>
@@ -971,6 +1306,12 @@
       <c r="A55">
         <v>54</v>
       </c>
+      <c r="B55" s="1">
+        <v>274</v>
+      </c>
+      <c r="C55" s="1">
+        <v>2</v>
+      </c>
       <c r="D55" t="s">
         <v>5</v>
       </c>
@@ -982,6 +1323,12 @@
       <c r="A56">
         <v>55</v>
       </c>
+      <c r="B56" s="1">
+        <v>276</v>
+      </c>
+      <c r="C56" s="1">
+        <v>6</v>
+      </c>
       <c r="D56" t="s">
         <v>5</v>
       </c>
@@ -993,6 +1340,12 @@
       <c r="A57">
         <v>56</v>
       </c>
+      <c r="B57" s="1">
+        <v>282</v>
+      </c>
+      <c r="C57" s="1">
+        <v>4</v>
+      </c>
       <c r="D57" t="s">
         <v>5</v>
       </c>
@@ -1004,6 +1357,12 @@
       <c r="A58">
         <v>57</v>
       </c>
+      <c r="B58" s="1">
+        <v>286</v>
+      </c>
+      <c r="C58" s="1">
+        <v>6</v>
+      </c>
       <c r="D58" t="s">
         <v>5</v>
       </c>
@@ -1015,6 +1374,12 @@
       <c r="A59">
         <v>58</v>
       </c>
+      <c r="B59" s="1">
+        <v>292</v>
+      </c>
+      <c r="C59" s="1">
+        <v>2</v>
+      </c>
       <c r="D59" t="s">
         <v>5</v>
       </c>
@@ -1026,6 +1391,12 @@
       <c r="A60">
         <v>59</v>
       </c>
+      <c r="B60" s="1">
+        <v>294</v>
+      </c>
+      <c r="C60" s="1">
+        <v>6</v>
+      </c>
       <c r="D60" t="s">
         <v>5</v>
       </c>
@@ -1037,6 +1408,12 @@
       <c r="A61">
         <v>60</v>
       </c>
+      <c r="B61" s="1">
+        <v>300</v>
+      </c>
+      <c r="C61" s="1">
+        <v>6</v>
+      </c>
       <c r="D61" t="s">
         <v>5</v>
       </c>
@@ -1048,6 +1425,12 @@
       <c r="A62">
         <v>61</v>
       </c>
+      <c r="B62" s="1">
+        <v>306</v>
+      </c>
+      <c r="C62" s="1">
+        <v>6</v>
+      </c>
       <c r="D62" t="s">
         <v>6</v>
       </c>
@@ -1059,6 +1442,12 @@
       <c r="A63">
         <v>62</v>
       </c>
+      <c r="B63" s="1">
+        <v>312</v>
+      </c>
+      <c r="C63" s="1">
+        <v>8</v>
+      </c>
       <c r="D63" t="s">
         <v>6</v>
       </c>
@@ -1070,6 +1459,12 @@
       <c r="A64">
         <v>63</v>
       </c>
+      <c r="B64" s="1">
+        <v>320</v>
+      </c>
+      <c r="C64" s="1">
+        <v>6</v>
+      </c>
       <c r="D64" t="s">
         <v>6</v>
       </c>
@@ -1081,6 +1476,12 @@
       <c r="A65">
         <v>64</v>
       </c>
+      <c r="B65" s="1">
+        <v>326</v>
+      </c>
+      <c r="C65" s="1">
+        <v>6</v>
+      </c>
       <c r="D65" t="s">
         <v>6</v>
       </c>
@@ -1092,6 +1493,12 @@
       <c r="A66">
         <v>65</v>
       </c>
+      <c r="B66" s="1">
+        <v>332</v>
+      </c>
+      <c r="C66" s="1">
+        <v>6</v>
+      </c>
       <c r="D66" t="s">
         <v>6</v>
       </c>
@@ -1103,6 +1510,12 @@
       <c r="A67">
         <v>66</v>
       </c>
+      <c r="B67" s="1">
+        <v>338</v>
+      </c>
+      <c r="C67" s="1">
+        <v>6</v>
+      </c>
       <c r="D67" t="s">
         <v>6</v>
       </c>
@@ -1114,6 +1527,12 @@
       <c r="A68">
         <v>67</v>
       </c>
+      <c r="B68" s="1">
+        <v>344</v>
+      </c>
+      <c r="C68" s="1">
+        <v>6</v>
+      </c>
       <c r="D68" t="s">
         <v>6</v>
       </c>
@@ -1124,6 +1543,12 @@
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
+      </c>
+      <c r="B69" s="1">
+        <v>350</v>
+      </c>
+      <c r="C69" s="1">
+        <v>10</v>
       </c>
       <c r="D69" t="s">
         <v>6</v>

</xml_diff>